<commit_message>
update scrape files + scrape results
</commit_message>
<xml_diff>
--- a/slurs.xlsx
+++ b/slurs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>racial slurs (from Jaki and De Smedt 2019)</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>Burka-Frauen</t>
-  </si>
-  <si>
-    <t>Mutombo</t>
-  </si>
-  <si>
-    <t>Bongo</t>
   </si>
   <si>
     <t>Kloneger</t>
@@ -422,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A26"/>
+  <dimension ref="A2:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -465,7 +459,7 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -473,74 +467,64 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>